<commit_message>
feat: make basic treemapping.
</commit_message>
<xml_diff>
--- a/example0.xlsx
+++ b/example0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>Garza</t>
+  </si>
+  <si>
+    <t>Duval</t>
+  </si>
+  <si>
+    <t>Zapata</t>
+  </si>
+  <si>
+    <t>Jim Hogg</t>
+  </si>
+  <si>
+    <t>Starr</t>
+  </si>
+  <si>
+    <t>McMullen</t>
+  </si>
+  <si>
+    <t>Furman</t>
+  </si>
+  <si>
+    <t>Atascosa</t>
+  </si>
+  <si>
+    <t>Bexar</t>
+  </si>
+  <si>
+    <t>Guadalupe</t>
   </si>
 </sst>
 </file>
@@ -370,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,6 +437,118 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>215</v>
+      </c>
+      <c r="C3">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>214</v>
+      </c>
+      <c r="C4">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>340</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>182</v>
+      </c>
+      <c r="C7">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>4680</v>
+      </c>
+      <c r="C8">
+        <v>1951</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>7664</v>
+      </c>
+      <c r="C9">
+        <v>3183</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>9493</v>
+      </c>
+      <c r="C10">
+        <v>5554</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>